<commit_message>
style: footer and login style added
</commit_message>
<xml_diff>
--- a/src/assets/Modelo para envio.xlsx
+++ b/src/assets/Modelo para envio.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ProdList\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ProdList\src\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E6898222-1133-4BCC-86C2-4DEA906959F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CC36789-D7CE-4FE5-93CA-67F8B27E954D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{EFA05852-0897-4C01-B187-C5847CF017FE}"/>
   </bookViews>
@@ -38,16 +38,16 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
-    <t>Produto</t>
+    <t>Title</t>
   </si>
   <si>
-    <t>Descrição</t>
+    <t>Description</t>
   </si>
   <si>
-    <t>Preço</t>
+    <t>Price</t>
   </si>
   <si>
-    <t>Quantidade</t>
+    <t>Quantity</t>
   </si>
 </sst>
 </file>
@@ -106,10 +106,10 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{59B54967-18FB-428B-BD53-D6AADE371307}" name="Tabela1" displayName="Tabela1" ref="A1:D2" totalsRowShown="0">
   <autoFilter ref="A1:D2" xr:uid="{59B54967-18FB-428B-BD53-D6AADE371307}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{83AF2AC9-92B0-4936-A41A-6EE54A309AEB}" name="Produto"/>
-    <tableColumn id="2" xr3:uid="{69CC7232-BD91-4E10-9CD0-1C39640ABEE0}" name="Descrição"/>
-    <tableColumn id="3" xr3:uid="{DCB8AA77-C56F-4A3F-B07A-CE15A4F4C569}" name="Preço"/>
-    <tableColumn id="4" xr3:uid="{F4E86604-7D05-4A61-A744-A94878482836}" name="Quantidade"/>
+    <tableColumn id="1" xr3:uid="{83AF2AC9-92B0-4936-A41A-6EE54A309AEB}" name="Title"/>
+    <tableColumn id="2" xr3:uid="{69CC7232-BD91-4E10-9CD0-1C39640ABEE0}" name="Description"/>
+    <tableColumn id="3" xr3:uid="{DCB8AA77-C56F-4A3F-B07A-CE15A4F4C569}" name="Price"/>
+    <tableColumn id="4" xr3:uid="{F4E86604-7D05-4A61-A744-A94878482836}" name="Quantity"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>

</xml_diff>